<commit_message>
Revert "fix: v8 ③탭 DOI-제목 불일치 수정 — CrossRef 기반 제목 교체 (55건)"
This reverts commit 4cd8625d189222eba819ee575b3e8b9e1cd56d41.
</commit_message>
<xml_diff>
--- a/data/templates/human_review_sheet_v8.xlsx
+++ b/data/templates/human_review_sheet_v8.xlsx
@@ -28113,7 +28113,7 @@
       </c>
       <c r="C3" s="37" t="inlineStr">
         <is>
-          <t>Inteligencia artificial en la transformación del proceso enseñanza-aprendizaje</t>
+          <t>Artificial Intelligence in the Transformation of the Teaching-Learning Process; Inteligencia artificial en la transformación del proceso enseñanza-aprendizaje</t>
         </is>
       </c>
       <c r="D3" s="36" t="n">
@@ -28159,7 +28159,7 @@
       </c>
       <c r="C4" s="37" t="inlineStr">
         <is>
-          <t>An expectancy value theory (EVT) based instrument for measuring student perceptions of generative AI</t>
+          <t>Artificial Intelligence (AI) applications and usage among the LIS professionals of Pakistan</t>
         </is>
       </c>
       <c r="D4" s="36" t="n">
@@ -28205,7 +28205,7 @@
       </c>
       <c r="C5" s="37" t="inlineStr">
         <is>
-          <t>Artificial Intelligence (AI) applications and usage among the LIS professionals of Pakistan</t>
+          <t>Perceptions of Higher Education Students towards ChatGPT Usage</t>
         </is>
       </c>
       <c r="D5" s="36" t="n">
@@ -28251,7 +28251,7 @@
       </c>
       <c r="C6" s="37" t="inlineStr">
         <is>
-          <t>The Role of Artificial Intelligence Autonomy in Higher Education: A Uses and Gratification Perspective</t>
+          <t>AI Integration in Higher Education: Trends and Implications from Saudi Arabia</t>
         </is>
       </c>
       <c r="D6" s="36" t="n">
@@ -28297,7 +28297,7 @@
       </c>
       <c r="C7" s="37" t="inlineStr">
         <is>
-          <t>Perceptions of Higher Education Students towards ChatGPT Usage</t>
+          <t>Artificial intelligence readiness among healthcare students in Nigeria: A cross-sectional study assessing knowledge gaps, exposure, and adoption willingness</t>
         </is>
       </c>
       <c r="D7" s="36" t="n">
@@ -28343,7 +28343,7 @@
       </c>
       <c r="C8" s="37" t="inlineStr">
         <is>
-          <t>AI Integration in Higher Education: Trends and Implications from Saudi Arabia</t>
+          <t>Academic self-efficacy and dependence on artificial intelligence in a sample of university students; Autoeficácia acadêmica e dependência da inteligência artificial em uma amostra de estudantes universitários; Autoeficacia académica y dependencia de la inteligencia artificial en una muestra de estudiantes universitarios</t>
         </is>
       </c>
       <c r="D8" s="36" t="n">
@@ -28389,7 +28389,7 @@
       </c>
       <c r="C9" s="37" t="inlineStr">
         <is>
-          <t>Artificial intelligence readiness among healthcare students in Nigeria: A cross-sectional study assessing knowledge gaps, exposure, and adoption willingness</t>
+          <t>The Double-Edged Sword Effect of Interaction Frequency with AI on College Students: The Moderating Role of Peer Support</t>
         </is>
       </c>
       <c r="D9" s="36" t="n">
@@ -28435,7 +28435,7 @@
       </c>
       <c r="C10" s="37" t="inlineStr">
         <is>
-          <t>Academic self-efficacy and dependence on artificial intelligence in a sample of university students</t>
+          <t>Knowledge and Perceptions of AI Among Medical Students in Morocco: Cross-Sectional Study</t>
         </is>
       </c>
       <c r="D10" s="36" t="n">
@@ -28481,7 +28481,7 @@
       </c>
       <c r="C11" s="37" t="inlineStr">
         <is>
-          <t>The Double-Edged Sword Effect of Interaction Frequency with AI on College Students: The Moderating Role of Peer Support</t>
+          <t>Will Teacher-AI Collaboration Enhance Teaching Engagement?</t>
         </is>
       </c>
       <c r="D11" s="36" t="n">
@@ -28527,7 +28527,7 @@
       </c>
       <c r="C12" s="37" t="inlineStr">
         <is>
-          <t>Generative AI and academic scientists in US universities: Perception, experience, and adoption intentions</t>
+          <t>Personality correlates of academic use of generative artificial intelligence and its outcomes: does fairness matter?</t>
         </is>
       </c>
       <c r="D12" s="36" t="n">
@@ -28573,7 +28573,7 @@
       </c>
       <c r="C13" s="37" t="inlineStr">
         <is>
-          <t>Knowledge and Perceptions of AI Among Medical Students in Morocco: Cross-Sectional Study</t>
+          <t>Attitudes of medical school students toward artificial intelligence in medical education: A survey study</t>
         </is>
       </c>
       <c r="D13" s="36" t="n">
@@ -28619,7 +28619,7 @@
       </c>
       <c r="C14" s="37" t="inlineStr">
         <is>
-          <t>Will Teacher-AI Collaboration Enhance Teaching Engagement?</t>
+          <t>Classroom innovation atmosphere and student creativity: the roles of AI technology application, intrinsic motivation, and self-efficacy</t>
         </is>
       </c>
       <c r="D14" s="36" t="n">
@@ -28665,7 +28665,7 @@
       </c>
       <c r="C15" s="37" t="inlineStr">
         <is>
-          <t>Análisis sobre el uso de las herramientas de inteligencia artificial interactiva en el entorno universitario</t>
+          <t>A catalyst for education? A study on the impact of artificial intelligence assisted learning in painting courses on college students' continuous learning intention</t>
         </is>
       </c>
       <c r="D15" s="36" t="n">
@@ -28711,7 +28711,7 @@
       </c>
       <c r="C16" s="37" t="inlineStr">
         <is>
-          <t>Personality correlates of academic use of generative artificial intelligence and its outcomes: does fairness matter?</t>
+          <t>Effects and acceptance of precision education in an AI-supported smart learning environment</t>
         </is>
       </c>
       <c r="D16" s="36" t="n">
@@ -28803,7 +28803,7 @@
       </c>
       <c r="C18" s="37" t="inlineStr">
         <is>
-          <t>Classroom innovation atmosphere and student creativity: the roles of AI technology application, intrinsic motivation, and self-efficacy</t>
+          <t>Use of ChatGPT at University as a Tool for Complex Thinking: Students' Perceived Usefulness</t>
         </is>
       </c>
       <c r="D18" s="36" t="n">
@@ -28849,7 +28849,7 @@
       </c>
       <c r="C19" s="37" t="inlineStr">
         <is>
-          <t>Enhancing the use of artificial intelligence in architectural education – case study Saudi Arabia</t>
+          <t>Students' adoption of AI-based teacher-bots (T-bots) for learning in higher education</t>
         </is>
       </c>
       <c r="D19" s="36" t="n">
@@ -28895,7 +28895,7 @@
       </c>
       <c r="C20" s="37" t="inlineStr">
         <is>
-          <t>A catalyst for education? A study on the impact of artificial intelligence assisted learning in painting courses on college students' continuous learning intention</t>
+          <t>Examining the influence of individual-level cultural values on CFL learners’ acceptance of ChatGPT for Chinese learning</t>
         </is>
       </c>
       <c r="D20" s="36" t="n">
@@ -28941,7 +28941,7 @@
       </c>
       <c r="C21" s="37" t="inlineStr">
         <is>
-          <t>Attitudes and Readiness for Artificial Intelligence Adoption Among Nursing Students in Saudi Arabia: A Cross-Sectional Study</t>
+          <t>Factors influencing the acceptance and use of ChatGPT among English as a foreign language learners in Saudi Arabia</t>
         </is>
       </c>
       <c r="D21" s="36" t="n">
@@ -28987,7 +28987,7 @@
       </c>
       <c r="C22" s="37" t="inlineStr">
         <is>
-          <t>The adoption of artificial intelligence applications in education</t>
+          <t>The TOP drivers of academics' adoption of ChatGPT in teaching</t>
         </is>
       </c>
       <c r="D22" s="36" t="n">
@@ -29033,7 +29033,7 @@
       </c>
       <c r="C23" s="37" t="inlineStr">
         <is>
-          <t>How do Chinese undergraduates harness the potential of appraisal and emotions in generative AI-Powered learning? A multigroup analysis based on appraisal theory</t>
+          <t>Exploring factors that influence graduate students' intention to use generative artificial intelligence in academic research: PLS-SEM and fsQCA methods</t>
         </is>
       </c>
       <c r="D23" s="36" t="n">
@@ -29079,7 +29079,7 @@
       </c>
       <c r="C24" s="37" t="inlineStr">
         <is>
-          <t>The Dual Impact of AI Adoption on College Students’ Academic Performance in Music Education: Evidence from China</t>
+          <t>In GenAI we trust: An investigation of university students' reliance on and resistance to generative AI in language learning</t>
         </is>
       </c>
       <c r="D24" s="36" t="n">
@@ -29125,7 +29125,7 @@
       </c>
       <c r="C25" s="37" t="inlineStr">
         <is>
-          <t>Effects and acceptance of precision education in an AI-supported smart learning environment</t>
+          <t>The relationship between students' self-regulated learning skills and technology acceptance of GenAI</t>
         </is>
       </c>
       <c r="D25" s="36" t="n">
@@ -29171,7 +29171,7 @@
       </c>
       <c r="C26" s="37" t="inlineStr">
         <is>
-          <t>Exploring the attitude and use of GenAI-image among art and design college students based on TAM and SDT</t>
+          <t>Measures of learner-generative ai relationships</t>
         </is>
       </c>
       <c r="D26" s="36" t="n">
@@ -29217,7 +29217,7 @@
       </c>
       <c r="C27" s="37" t="inlineStr">
         <is>
-          <t>Use of ChatGPT at University as a Tool for Complex Thinking: Students’ Perceived Usefulness</t>
+          <t>Mindsets Matter: A Mediation Analysis of the Role of a Technological Growth Mindset in Generative Artificial Intelligence Usage in Higher Education</t>
         </is>
       </c>
       <c r="D27" s="36" t="n">
@@ -29263,7 +29263,7 @@
       </c>
       <c r="C28" s="37" t="inlineStr">
         <is>
-          <t>Students' adoption of AI-based teacher-bots (T-bots) for learning in higher education</t>
+          <t>ChatGPT for Educational Purposes: Investigating the Impact of Knowledge Management Factors on Student Satisfaction and Continuous Usage</t>
         </is>
       </c>
       <c r="D28" s="36" t="n">
@@ -29309,7 +29309,7 @@
       </c>
       <c r="C29" s="37" t="inlineStr">
         <is>
-          <t>Examining the influence of individual-level cultural values on CFL learners’ acceptance of ChatGPT for Chinese learning</t>
+          <t>Investigating Korean College EFL Learners’ Perceptions and Intentions toward AI-Enabled Language Learning Applications*</t>
         </is>
       </c>
       <c r="D29" s="36" t="n">
@@ -29355,7 +29355,7 @@
       </c>
       <c r="C30" s="37" t="inlineStr">
         <is>
-          <t>Factors influencing the acceptance and use of ChatGPT among English as a foreign language learners in Saudi Arabia</t>
+          <t>Navigating AI integration in higher education: assessing the impact of assessment formats and motivation types on students' AI usage intentions</t>
         </is>
       </c>
       <c r="D30" s="36" t="n">
@@ -29401,7 +29401,7 @@
       </c>
       <c r="C31" s="37" t="inlineStr">
         <is>
-          <t>The “TOP” drivers of academics’ adoption of ChatGPT in teaching</t>
+          <t>AI-assisted learning: an empirical study on student application behavior</t>
         </is>
       </c>
       <c r="D31" s="36" t="n">
@@ -29447,7 +29447,7 @@
       </c>
       <c r="C32" s="37" t="inlineStr">
         <is>
-          <t>Exploring factors that influence graduate students’ intention to use generative artificial intelligence in academic research: PLS-SEM and fsQCA methods</t>
+          <t>Is Anxiety Affecting the Adoption of ChatGPT in University Teaching? A Gender Perspective</t>
         </is>
       </c>
       <c r="D32" s="36" t="n">
@@ -29493,7 +29493,7 @@
       </c>
       <c r="C33" s="37" t="inlineStr">
         <is>
-          <t>In GenAI we trust: An investigation of university students’ reliance on and resistance to generative AI in language learning</t>
+          <t>The Role of ChatGPT in English Language Learning: A Hedonic Motivation Perspective on Student Adoption in Chinese Universities</t>
         </is>
       </c>
       <c r="D33" s="36" t="n">
@@ -29539,7 +29539,7 @@
       </c>
       <c r="C34" s="37" t="inlineStr">
         <is>
-          <t>The relationship between students’ self-regulated learning skills and technology acceptance of GenAI</t>
+          <t>Acceptance of Educational Artificial Intelligence by Teachers and Its Relationship with Some Variables and Pedagogical Beliefs</t>
         </is>
       </c>
       <c r="D34" s="36" t="n">
@@ -29585,7 +29585,7 @@
       </c>
       <c r="C35" s="37" t="inlineStr">
         <is>
-          <t>Measures of learner-generative ai relationships</t>
+          <t>AI in medical education: the moderating role of the chilling effect and STARA awareness</t>
         </is>
       </c>
       <c r="D35" s="36" t="n">
@@ -29631,7 +29631,7 @@
       </c>
       <c r="C36" s="37" t="inlineStr">
         <is>
-          <t>Mindsets Matter: A Mediation Analysis of the Role of a Technological Growth Mindset in Generative Artificial Intelligence Usage in Higher Education</t>
+          <t>Examining factors influencing university students' perceptions of AI technologies in academic writing</t>
         </is>
       </c>
       <c r="D36" s="36" t="n">
@@ -29677,7 +29677,7 @@
       </c>
       <c r="C37" s="37" t="inlineStr">
         <is>
-          <t>ChatGPT for Educational Purposes: Investigating the Impact of Knowledge Management Factors on Student Satisfaction and Continuous Usage</t>
+          <t>Exploring indian students’ perception, behavioral intentions, and motivation for learning with chatgpt</t>
         </is>
       </c>
       <c r="D37" s="36" t="n">
@@ -29723,7 +29723,7 @@
       </c>
       <c r="C38" s="37" t="inlineStr">
         <is>
-          <t>Investigating Korean College EFL Learners’ Perceptions and Intentions toward AI-Enabled Language Learning Applications</t>
+          <t>Understanding the role of AI in Malaysian higher education curricula: an analysis of student perceptions</t>
         </is>
       </c>
       <c r="D38" s="36" t="n">
@@ -29769,7 +29769,7 @@
       </c>
       <c r="C39" s="37" t="inlineStr">
         <is>
-          <t>Navigating AI integration in higher education: assessing the impact of assessment formats and motivation types on students’ AI usage intentions</t>
+          <t>Lecturers' pathways to integrating artificial intelligence in business and economics curricula</t>
         </is>
       </c>
       <c r="D39" s="36" t="n">
@@ -29815,7 +29815,7 @@
       </c>
       <c r="C40" s="37" t="inlineStr">
         <is>
-          <t>AI-assisted learning: an empirical study on student application behavior</t>
+          <t>Exploring the role of generative artificial intelligence (ChatGPT) adoption in digital social entrepreneurship: a serial mediation model</t>
         </is>
       </c>
       <c r="D40" s="36" t="n">
@@ -29861,7 +29861,7 @@
       </c>
       <c r="C41" s="37" t="inlineStr">
         <is>
-          <t>Is Anxiety Affecting the Adoption of ChatGPT in University Teaching? A Gender Perspective</t>
+          <t>AI-driven academic engagement in fine arts education: the chain-mediating roles of self-efficacy and achievement emotions</t>
         </is>
       </c>
       <c r="D41" s="36" t="n">
@@ -29907,7 +29907,7 @@
       </c>
       <c r="C42" s="37" t="inlineStr">
         <is>
-          <t>The Role of ChatGPT in English Language Learning: A Hedonic Motivation Perspective on Student Adoption in Chinese Universities</t>
+          <t>Participant or spectator? Comprehending the willingness of faculty to use intelligent tutoring systems in the artificial intelligence era</t>
         </is>
       </c>
       <c r="D42" s="36" t="n">
@@ -29953,7 +29953,7 @@
       </c>
       <c r="C43" s="37" t="inlineStr">
         <is>
-          <t>Acceptance of Educational Artificial Intelligence by Teachers and Its Relationship with Some Variables and Pedagogical Beliefs</t>
+          <t>Analysis of college students' attitudes toward the use of ChatGPT in their academic activities: effect of intent to use, verification of information and responsible use</t>
         </is>
       </c>
       <c r="D43" s="36" t="n">
@@ -29999,7 +29999,7 @@
       </c>
       <c r="C44" s="37" t="inlineStr">
         <is>
-          <t>AI in medical education: the moderating role of the chilling effect and STARA awareness</t>
+          <t>EXPLORING STUDENTS' AND FACULTY'S KNOWLEDGE, ATTITUDES, AND PERCEPTIONS TOWARDS CHATGPT: A CROSS-SECTIONAL EMPIRICAL STUDY</t>
         </is>
       </c>
       <c r="D44" s="36" t="n">
@@ -30045,7 +30045,7 @@
       </c>
       <c r="C45" s="37" t="inlineStr">
         <is>
-          <t>Examining factors influencing university students’ perceptions of AI technologies in academic writing</t>
+          <t>Unlocking AI-Powered Tools Adoption among University Students: A Fuzzy-Set Approach</t>
         </is>
       </c>
       <c r="D45" s="36" t="n">
@@ -30091,7 +30091,7 @@
       </c>
       <c r="C46" s="37" t="inlineStr">
         <is>
-          <t>Exploring Indian Students’ Perception, Behavioral Intentions, and Motivation for Learning with ChatGPT</t>
+          <t>Who will benefit from AIGC: An empirical study on the intentions to use artificial intelligence generated content in higher education</t>
         </is>
       </c>
       <c r="D46" s="36" t="n">
@@ -30137,7 +30137,7 @@
       </c>
       <c r="C47" s="37" t="inlineStr">
         <is>
-          <t>Understanding the role of AI in Malaysian higher education curricula: an analysis of student perceptions</t>
+          <t>Comparing Lecturers and Students Attitude towards the Role of Generative Artificial Intelligence Systems in Foreign Language Teaching and Learning</t>
         </is>
       </c>
       <c r="D47" s="36" t="n">
@@ -30183,7 +30183,7 @@
       </c>
       <c r="C48" s="37" t="inlineStr">
         <is>
-          <t>Lecturers’ pathways to integrating artificial intelligence in business and economics curricula</t>
+          <t>Predictors of Pre-Service EFL Teachers' Predisposition Towards AI Adoption in Language Teaching</t>
         </is>
       </c>
       <c r="D48" s="36" t="n">
@@ -30229,7 +30229,7 @@
       </c>
       <c r="C49" s="37" t="inlineStr">
         <is>
-          <t>Exploring the role of generative artificial intelligence (ChatGPT) adoption in digital social entrepreneurship: a serial mediation model</t>
+          <t>Students’ Perceptions of Artificial Intelligence in Academic Writing: A Case at A University in Vietnam</t>
         </is>
       </c>
       <c r="D49" s="36" t="n">
@@ -30275,7 +30275,7 @@
       </c>
       <c r="C50" s="37" t="inlineStr">
         <is>
-          <t>AI-driven academic engagement in fine arts education: the chain-mediating roles of self-efficacy and achievement emotions</t>
+          <t>Examining ChatGPT adoption among educators in higher educational institutions using extended UTAUT model</t>
         </is>
       </c>
       <c r="D50" s="36" t="n">
@@ -30321,7 +30321,7 @@
       </c>
       <c r="C51" s="37" t="inlineStr">
         <is>
-          <t>Participant or spectator? Comprehending the willingness of faculty to use intelligent tutoring systems in the artificial intelligence era</t>
+          <t>Impact of perceived ease of use and perceived usefulness of humanoid robots on students' intention to use</t>
         </is>
       </c>
       <c r="D51" s="36" t="n">
@@ -30367,7 +30367,7 @@
       </c>
       <c r="C52" s="37" t="inlineStr">
         <is>
-          <t>Analysis of college students' attitudes toward the use of ChatGPT in their academic activities: effect of intent to use, verification of information and responsible use</t>
+          <t>Developing a New Model of Using Artificial Intelligence and Postmodern Arts in Visual Arts and Design Courses (VADC) Among University Students</t>
         </is>
       </c>
       <c r="D52" s="36" t="n">
@@ -30413,7 +30413,7 @@
       </c>
       <c r="C53" s="37" t="inlineStr">
         <is>
-          <t>Exploring Students’ and Faculty’s Knowledge, Attitudes, and Perceptions Towards ChatGPT: A Cross-Sectional Empirical Study</t>
+          <t>Revolutionizing education: Artificial intelligence empowered learning in higher education</t>
         </is>
       </c>
       <c r="D53" s="36" t="n">
@@ -30459,7 +30459,7 @@
       </c>
       <c r="C54" s="37" t="inlineStr">
         <is>
-          <t>Unlocking AI-Powered Tools Adoption among University Students: A Fuzzy-Set Approach</t>
+          <t>Conversational agent-based guidance: examining the effect of chatbot usage frequency and satisfaction on visual design self-efficacy, engagement, satisfaction, and learner autonomy</t>
         </is>
       </c>
       <c r="D54" s="36" t="n">
@@ -30505,7 +30505,7 @@
       </c>
       <c r="C55" s="37" t="inlineStr">
         <is>
-          <t>Who will benefit from AIGC: An empirical study on the intentions to use artificial intelligence generated content in higher education</t>
+          <t>Assessing attitudes and impact of AI integration in higher education</t>
         </is>
       </c>
       <c r="D55" s="36" t="n">
@@ -30551,7 +30551,7 @@
       </c>
       <c r="C56" s="37" t="inlineStr">
         <is>
-          <t>Comparing Lecturers and Students Attitude towards the Role of Generative Artificial Intelligence Systems in Foreign Language Teaching and Learning</t>
+          <t>Language Attitude and GenAI Attitude of Struggling EFL Learners: A Moderated Mediation Model of Enjoyment and Anxiety</t>
         </is>
       </c>
       <c r="D56" s="36" t="n">
@@ -30597,7 +30597,7 @@
       </c>
       <c r="C57" s="37" t="inlineStr">
         <is>
-          <t>Predictors of Pre-Service EFL Teachers’ Predisposition Towards AI Adoption in Language Teaching</t>
+          <t>Using Generative AI in nursing education: Students' perceptions</t>
         </is>
       </c>
       <c r="D57" s="36" t="n">
@@ -30689,7 +30689,7 @@
       </c>
       <c r="C59" s="37" t="inlineStr">
         <is>
-          <t>Examining ChatGPT adoption among educators in higher educational institutions using extended UTAUT model</t>
+          <t>AIDUA (artificial intelligence device use and acceptance) model to assess the acceptance of AI in the learning practices of higher education students</t>
         </is>
       </c>
       <c r="D59" s="36" t="n">
@@ -35796,8 +35796,12 @@
           <t>📋 UTAUT2 구성개념 처리 근거</t>
         </is>
       </c>
-    </row>
-    <row r="67"/>
+      <c r="B66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+    </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
@@ -35846,15 +35850,22 @@
         </is>
       </c>
     </row>
-    <row r="72"/>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+    </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
           <t>📋 AI-Specific 4개 Construct 포함 근거</t>
         </is>
       </c>
-    </row>
-    <row r="74"/>
+      <c r="B73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+    </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
@@ -35915,13 +35926,17 @@
         </is>
       </c>
     </row>
-    <row r="80"/>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+    </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
           <t>🔑 TAM-UTAUT 교집합 (4개)</t>
         </is>
       </c>
+      <c r="B81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">

</xml_diff>

<commit_message>
fix: v8 ③탭 DOI 교정 + 코딩 재배치 (sim≥0.80 기준)
Tab3 전수조사 결과:
- DOI 132건 교체 (제목 기반 CrossRef 검색으로 올바른 DOI 매칭)
- 코딩 47건 올바른 행으로 재배치 (충돌 0건)
- 외부 논문 10건 코딩 삭제 (#2,4,10,13,15,17,19,21,22,56)
  → DOI가 가리킨 논문이 Tab3에 존재하지 않음
- 미코딩 11건 (#11,47,49-57): 올바른 DOI가 기존 시트에 없던 행

Tab1(200건), Tab2(367건): 정상 확인 (실질 불일치 0건)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/templates/human_review_sheet_v8.xlsx
+++ b/data/templates/human_review_sheet_v8.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -125,12 +125,8 @@
       <sz val="9"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FF0000"/>
-    </font>
   </fonts>
-  <fills count="22">
+  <fills count="19">
     <fill>
       <patternFill/>
     </fill>
@@ -237,24 +233,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF57F17"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0099FF99"/>
-        <bgColor rgb="0099FF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF9999"/>
-        <bgColor rgb="00FF9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -448,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -579,20 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28028,7 +27992,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -28234,17 +28198,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J4" s="48" t="inlineStr">
+      <c r="J4" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K4" s="48" t="inlineStr">
+      <c r="K4" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L4" s="49" t="n"/>
+      <c r="L4" s="28" t="n"/>
     </row>
     <row r="5" ht="28" customHeight="1">
       <c r="A5" s="36" t="n">
@@ -28288,17 +28252,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J5" s="48" t="inlineStr">
+      <c r="J5" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K5" s="48" t="inlineStr">
+      <c r="K5" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L5" s="49" t="n"/>
+      <c r="L5" s="28" t="n"/>
     </row>
     <row r="6" ht="28" customHeight="1">
       <c r="A6" s="36" t="n">
@@ -28342,17 +28306,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J6" s="48" t="inlineStr">
+      <c r="J6" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K6" s="48" t="inlineStr">
+      <c r="K6" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L6" s="49" t="n"/>
+      <c r="L6" s="28" t="n"/>
     </row>
     <row r="7" ht="28" customHeight="1">
       <c r="A7" s="36" t="n">
@@ -28396,17 +28360,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J7" s="50" t="inlineStr">
+      <c r="J7" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K7" s="50" t="inlineStr">
+      <c r="K7" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L7" s="51" t="n"/>
+      <c r="L7" s="28" t="n"/>
     </row>
     <row r="8" ht="28" customHeight="1">
       <c r="A8" s="36" t="n">
@@ -28450,17 +28414,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J8" s="48" t="inlineStr">
+      <c r="J8" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K8" s="48" t="inlineStr">
+      <c r="K8" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L8" s="49" t="n"/>
+      <c r="L8" s="28" t="n"/>
     </row>
     <row r="9" ht="28" customHeight="1">
       <c r="A9" s="36" t="n">
@@ -28504,17 +28468,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J9" s="48" t="inlineStr">
+      <c r="J9" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K9" s="48" t="inlineStr">
+      <c r="K9" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L9" s="49" t="n"/>
+      <c r="L9" s="28" t="n"/>
     </row>
     <row r="10" ht="28" customHeight="1">
       <c r="A10" s="36" t="n">
@@ -28558,17 +28522,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J10" s="48" t="inlineStr">
+      <c r="J10" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K10" s="48" t="inlineStr">
+      <c r="K10" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L10" s="49" t="n"/>
+      <c r="L10" s="28" t="n"/>
     </row>
     <row r="11" ht="28" customHeight="1">
       <c r="A11" s="36" t="n">
@@ -28612,17 +28576,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J11" s="48" t="inlineStr">
+      <c r="J11" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K11" s="48" t="inlineStr">
+      <c r="K11" s="27" t="inlineStr">
         <is>
           <t>E-FT1</t>
         </is>
       </c>
-      <c r="L11" s="49" t="n"/>
+      <c r="L11" s="28" t="n"/>
     </row>
     <row r="12" ht="28" customHeight="1">
       <c r="A12" s="36" t="n">
@@ -28666,17 +28630,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J12" s="48" t="inlineStr">
+      <c r="J12" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K12" s="48" t="inlineStr">
+      <c r="K12" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L12" s="49" t="n"/>
+      <c r="L12" s="28" t="n"/>
     </row>
     <row r="13" ht="28" customHeight="1">
       <c r="A13" s="36" t="n">
@@ -28766,17 +28730,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J14" s="48" t="inlineStr">
+      <c r="J14" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K14" s="48" t="inlineStr">
+      <c r="K14" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L14" s="49" t="n"/>
+      <c r="L14" s="28" t="n"/>
     </row>
     <row r="15" ht="28" customHeight="1">
       <c r="A15" s="36" t="n">
@@ -28820,17 +28784,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J15" s="48" t="inlineStr">
+      <c r="J15" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K15" s="48" t="inlineStr">
+      <c r="K15" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L15" s="49" t="n"/>
+      <c r="L15" s="28" t="n"/>
     </row>
     <row r="16" ht="28" customHeight="1">
       <c r="A16" s="36" t="n">
@@ -28874,13 +28838,13 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J16" s="48" t="inlineStr">
+      <c r="J16" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K16" s="48" t="n"/>
-      <c r="L16" s="49" t="n"/>
+      <c r="K16" s="27" t="n"/>
+      <c r="L16" s="28" t="n"/>
     </row>
     <row r="17" ht="28" customHeight="1">
       <c r="A17" s="36" t="n">
@@ -28924,13 +28888,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J17" s="48" t="n"/>
-      <c r="K17" s="48" t="inlineStr">
+      <c r="J17" s="27" t="n"/>
+      <c r="K17" s="27" t="inlineStr">
         <is>
           <t>E-FT6</t>
         </is>
       </c>
-      <c r="L17" s="49" t="n"/>
+      <c r="L17" s="28" t="n"/>
     </row>
     <row r="18" ht="28" customHeight="1">
       <c r="A18" s="36" t="n">
@@ -28974,13 +28938,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J18" s="48" t="inlineStr">
+      <c r="J18" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K18" s="48" t="n"/>
-      <c r="L18" s="49" t="n"/>
+      <c r="K18" s="27" t="n"/>
+      <c r="L18" s="28" t="n"/>
     </row>
     <row r="19" ht="28" customHeight="1">
       <c r="A19" s="36" t="n">
@@ -29024,13 +28988,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J19" s="48" t="inlineStr">
+      <c r="J19" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K19" s="48" t="n"/>
-      <c r="L19" s="49" t="n"/>
+      <c r="K19" s="27" t="n"/>
+      <c r="L19" s="28" t="n"/>
     </row>
     <row r="20" ht="28" customHeight="1">
       <c r="A20" s="36" t="n">
@@ -29074,13 +29038,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J20" s="48" t="inlineStr">
+      <c r="J20" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K20" s="48" t="n"/>
-      <c r="L20" s="49" t="n"/>
+      <c r="K20" s="27" t="n"/>
+      <c r="L20" s="28" t="n"/>
     </row>
     <row r="21" ht="28" customHeight="1">
       <c r="A21" s="36" t="n">
@@ -29124,13 +29088,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J21" s="48" t="inlineStr">
+      <c r="J21" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K21" s="48" t="n"/>
-      <c r="L21" s="49" t="n"/>
+      <c r="K21" s="27" t="n"/>
+      <c r="L21" s="28" t="n"/>
     </row>
     <row r="22" ht="28" customHeight="1">
       <c r="A22" s="36" t="n">
@@ -29174,21 +29138,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J22" s="50" t="inlineStr">
+      <c r="J22" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K22" s="50" t="inlineStr">
-        <is>
-          <t>E-FT2</t>
-        </is>
-      </c>
-      <c r="L22" s="51" t="inlineStr">
-        <is>
-          <t>[충돌] 소스#29: 판단=X, 코드=E-FT6;</t>
-        </is>
-      </c>
+      <c r="K22" s="27" t="inlineStr">
+        <is>
+          <t>E-FT6</t>
+        </is>
+      </c>
+      <c r="L22" s="28" t="n"/>
     </row>
     <row r="23" ht="28" customHeight="1">
       <c r="A23" s="36" t="n">
@@ -29232,13 +29192,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J23" s="48" t="inlineStr">
+      <c r="J23" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K23" s="48" t="n"/>
-      <c r="L23" s="49" t="n"/>
+      <c r="K23" s="27" t="n"/>
+      <c r="L23" s="28" t="n"/>
     </row>
     <row r="24" ht="28" customHeight="1">
       <c r="A24" s="36" t="n">
@@ -29282,13 +29242,13 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J24" s="48" t="inlineStr">
+      <c r="J24" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K24" s="48" t="n"/>
-      <c r="L24" s="49" t="n"/>
+      <c r="K24" s="27" t="n"/>
+      <c r="L24" s="28" t="n"/>
     </row>
     <row r="25" ht="28" customHeight="1">
       <c r="A25" s="36" t="n">
@@ -29332,17 +29292,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J25" s="48" t="inlineStr">
+      <c r="J25" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K25" s="48" t="inlineStr">
+      <c r="K25" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L25" s="49" t="n"/>
+      <c r="L25" s="28" t="n"/>
     </row>
     <row r="26" ht="28" customHeight="1">
       <c r="A26" s="36" t="n">
@@ -29386,17 +29346,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J26" s="50" t="inlineStr">
+      <c r="J26" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K26" s="50" t="inlineStr">
+      <c r="K26" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L26" s="51" t="n"/>
+      <c r="L26" s="28" t="n"/>
     </row>
     <row r="27" ht="28" customHeight="1">
       <c r="A27" s="36" t="n">
@@ -29440,21 +29400,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J27" s="50" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K27" s="50" t="inlineStr">
-        <is>
-          <t>E-FT2</t>
-        </is>
-      </c>
-      <c r="L27" s="51" t="inlineStr">
-        <is>
-          <t>[충돌] 소스#34: 판단=I, 코드=None;</t>
-        </is>
-      </c>
+      <c r="J27" s="27" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="K27" s="27" t="n"/>
+      <c r="L27" s="28" t="n"/>
     </row>
     <row r="28" ht="28" customHeight="1">
       <c r="A28" s="36" t="n">
@@ -29498,17 +29450,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J28" s="48" t="inlineStr">
+      <c r="J28" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K28" s="48" t="inlineStr">
+      <c r="K28" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L28" s="49" t="n"/>
+      <c r="L28" s="28" t="n"/>
     </row>
     <row r="29" ht="28" customHeight="1">
       <c r="A29" s="36" t="n">
@@ -29552,17 +29504,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J29" s="48" t="inlineStr">
+      <c r="J29" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K29" s="48" t="inlineStr">
+      <c r="K29" s="27" t="inlineStr">
         <is>
           <t>E-FT1</t>
         </is>
       </c>
-      <c r="L29" s="49" t="n"/>
+      <c r="L29" s="28" t="n"/>
     </row>
     <row r="30" ht="28" customHeight="1">
       <c r="A30" s="36" t="n">
@@ -29606,17 +29558,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J30" s="48" t="inlineStr">
+      <c r="J30" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K30" s="48" t="inlineStr">
+      <c r="K30" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L30" s="49" t="n"/>
+      <c r="L30" s="28" t="n"/>
     </row>
     <row r="31" ht="28" customHeight="1">
       <c r="A31" s="36" t="n">
@@ -29660,17 +29612,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J31" s="48" t="inlineStr">
+      <c r="J31" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K31" s="48" t="inlineStr">
+      <c r="K31" s="27" t="inlineStr">
         <is>
           <t>E-FT1</t>
         </is>
       </c>
-      <c r="L31" s="49" t="n"/>
+      <c r="L31" s="28" t="n"/>
     </row>
     <row r="32" ht="28" customHeight="1">
       <c r="A32" s="36" t="n">
@@ -29714,13 +29666,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J32" s="48" t="inlineStr">
+      <c r="J32" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K32" s="48" t="n"/>
-      <c r="L32" s="49" t="n"/>
+      <c r="K32" s="27" t="n"/>
+      <c r="L32" s="28" t="n"/>
     </row>
     <row r="33" ht="28" customHeight="1">
       <c r="A33" s="36" t="n">
@@ -29764,17 +29716,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J33" s="48" t="inlineStr">
+      <c r="J33" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K33" s="48" t="inlineStr">
+      <c r="K33" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L33" s="49" t="n"/>
+      <c r="L33" s="28" t="n"/>
     </row>
     <row r="34" ht="28" customHeight="1">
       <c r="A34" s="36" t="n">
@@ -29818,13 +29770,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J34" s="48" t="inlineStr">
+      <c r="J34" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K34" s="48" t="n"/>
-      <c r="L34" s="49" t="n"/>
+      <c r="K34" s="27" t="n"/>
+      <c r="L34" s="28" t="n"/>
     </row>
     <row r="35" ht="28" customHeight="1">
       <c r="A35" s="36" t="n">
@@ -29868,13 +29820,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J35" s="48" t="inlineStr">
+      <c r="J35" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K35" s="48" t="n"/>
-      <c r="L35" s="49" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="28" t="n"/>
     </row>
     <row r="36" ht="28" customHeight="1">
       <c r="A36" s="36" t="n">
@@ -29918,13 +29870,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J36" s="48" t="inlineStr">
+      <c r="J36" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K36" s="48" t="n"/>
-      <c r="L36" s="49" t="n"/>
+      <c r="K36" s="27" t="n"/>
+      <c r="L36" s="28" t="n"/>
     </row>
     <row r="37" ht="28" customHeight="1">
       <c r="A37" s="36" t="n">
@@ -29968,13 +29920,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J37" s="48" t="inlineStr">
+      <c r="J37" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K37" s="48" t="n"/>
-      <c r="L37" s="49" t="n"/>
+      <c r="K37" s="27" t="n"/>
+      <c r="L37" s="28" t="n"/>
     </row>
     <row r="38" ht="28" customHeight="1">
       <c r="A38" s="36" t="n">
@@ -30018,17 +29970,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J38" s="48" t="inlineStr">
+      <c r="J38" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K38" s="48" t="inlineStr">
+      <c r="K38" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L38" s="49" t="n"/>
+      <c r="L38" s="28" t="n"/>
     </row>
     <row r="39" ht="28" customHeight="1">
       <c r="A39" s="36" t="n">
@@ -30072,17 +30024,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J39" s="48" t="inlineStr">
+      <c r="J39" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K39" s="48" t="inlineStr">
+      <c r="K39" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L39" s="49" t="n"/>
+      <c r="L39" s="28" t="n"/>
     </row>
     <row r="40" ht="28" customHeight="1">
       <c r="A40" s="36" t="n">
@@ -30126,17 +30078,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J40" s="48" t="inlineStr">
+      <c r="J40" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K40" s="48" t="inlineStr">
+      <c r="K40" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L40" s="49" t="n"/>
+      <c r="L40" s="28" t="n"/>
     </row>
     <row r="41" ht="28" customHeight="1">
       <c r="A41" s="36" t="n">
@@ -30180,17 +30132,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J41" s="48" t="inlineStr">
+      <c r="J41" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K41" s="48" t="inlineStr">
+      <c r="K41" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L41" s="49" t="n"/>
+      <c r="L41" s="28" t="n"/>
     </row>
     <row r="42" ht="28" customHeight="1">
       <c r="A42" s="36" t="n">
@@ -30234,17 +30186,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J42" s="48" t="inlineStr">
+      <c r="J42" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K42" s="48" t="inlineStr">
+      <c r="K42" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L42" s="49" t="n"/>
+      <c r="L42" s="28" t="n"/>
     </row>
     <row r="43" ht="28" customHeight="1">
       <c r="A43" s="36" t="n">
@@ -30288,17 +30240,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J43" s="48" t="inlineStr">
+      <c r="J43" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K43" s="48" t="inlineStr">
+      <c r="K43" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L43" s="49" t="n"/>
+      <c r="L43" s="28" t="n"/>
     </row>
     <row r="44" ht="28" customHeight="1">
       <c r="A44" s="36" t="n">
@@ -30342,17 +30294,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J44" s="48" t="inlineStr">
+      <c r="J44" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K44" s="48" t="inlineStr">
+      <c r="K44" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L44" s="49" t="n"/>
+      <c r="L44" s="28" t="n"/>
     </row>
     <row r="45" ht="28" customHeight="1">
       <c r="A45" s="36" t="n">
@@ -30396,17 +30348,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J45" s="48" t="inlineStr">
+      <c r="J45" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K45" s="48" t="inlineStr">
+      <c r="K45" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L45" s="49" t="n"/>
+      <c r="L45" s="28" t="n"/>
     </row>
     <row r="46" ht="28" customHeight="1">
       <c r="A46" s="36" t="n">
@@ -30450,17 +30402,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J46" s="48" t="inlineStr">
+      <c r="J46" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K46" s="48" t="inlineStr">
+      <c r="K46" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L46" s="49" t="n"/>
+      <c r="L46" s="28" t="n"/>
     </row>
     <row r="47" ht="28" customHeight="1">
       <c r="A47" s="36" t="n">
@@ -30504,17 +30456,17 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J47" s="48" t="inlineStr">
+      <c r="J47" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K47" s="48" t="inlineStr">
+      <c r="K47" s="27" t="inlineStr">
         <is>
           <t>E-FT3</t>
         </is>
       </c>
-      <c r="L47" s="49" t="n"/>
+      <c r="L47" s="28" t="n"/>
     </row>
     <row r="48" ht="28" customHeight="1">
       <c r="A48" s="36" t="n">
@@ -30558,17 +30510,17 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J48" s="48" t="inlineStr">
+      <c r="J48" s="27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K48" s="48" t="inlineStr">
+      <c r="K48" s="27" t="inlineStr">
         <is>
           <t>E-FT2</t>
         </is>
       </c>
-      <c r="L48" s="49" t="n"/>
+      <c r="L48" s="28" t="n"/>
     </row>
     <row r="49" ht="28" customHeight="1">
       <c r="A49" s="36" t="n">
@@ -30658,13 +30610,13 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J50" s="48" t="inlineStr">
+      <c r="J50" s="27" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="K50" s="48" t="n"/>
-      <c r="L50" s="49" t="n"/>
+      <c r="K50" s="27" t="n"/>
+      <c r="L50" s="28" t="n"/>
     </row>
     <row r="51" ht="28" customHeight="1">
       <c r="A51" s="36" t="n">
@@ -30892,17 +30844,9 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J55" s="48" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K55" s="48" t="inlineStr">
-        <is>
-          <t>E-FT2</t>
-        </is>
-      </c>
-      <c r="L55" s="49" t="n"/>
+      <c r="J55" s="27" t="n"/>
+      <c r="K55" s="27" t="n"/>
+      <c r="L55" s="28" t="n"/>
     </row>
     <row r="56" ht="28" customHeight="1">
       <c r="A56" s="36" t="n">
@@ -31130,8 +31074,16 @@
           <t>uncertain+include</t>
         </is>
       </c>
-      <c r="J60" s="27" t="n"/>
-      <c r="K60" s="27" t="n"/>
+      <c r="J60" s="27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K60" s="27" t="inlineStr">
+        <is>
+          <t>E-FT2</t>
+        </is>
+      </c>
       <c r="L60" s="28" t="n"/>
     </row>
     <row r="61" ht="28" customHeight="1">
@@ -34626,17 +34578,9 @@
           <t>include+uncertain</t>
         </is>
       </c>
-      <c r="J136" s="48" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K136" s="48" t="inlineStr">
-        <is>
-          <t>E-FT2</t>
-        </is>
-      </c>
-      <c r="L136" s="49" t="n"/>
+      <c r="J136" s="27" t="n"/>
+      <c r="K136" s="27" t="n"/>
+      <c r="L136" s="28" t="n"/>
     </row>
     <row r="137" ht="28" customHeight="1">
       <c r="A137" s="36" t="n">
@@ -34953,164 +34897,6 @@
       <c r="J152" s="27" t="n"/>
       <c r="K152" s="27" t="n"/>
       <c r="L152" s="28" t="n"/>
-    </row>
-    <row r="154">
-      <c r="A154" s="52">
-        <f>== 외부 논문 코딩 (Tab3에 없는 DOI 기반 코딩) ===</f>
-        <v/>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="53" t="inlineStr">
-        <is>
-          <t>원래 #10</t>
-        </is>
-      </c>
-      <c r="B155" s="53" t="inlineStr">
-        <is>
-          <t>10.1371/journal.pone.0330416</t>
-        </is>
-      </c>
-      <c r="C155" s="53" t="inlineStr">
-        <is>
-          <t>Generative AI and academic scientists in US universities: Perception, experience</t>
-        </is>
-      </c>
-      <c r="D155" s="53" t="n"/>
-      <c r="E155" s="53" t="n"/>
-      <c r="F155" s="53" t="n"/>
-      <c r="G155" s="53" t="n"/>
-      <c r="H155" s="53" t="n"/>
-      <c r="I155" s="53" t="n"/>
-      <c r="J155" s="53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K155" s="53" t="inlineStr">
-        <is>
-          <t>E-FT1</t>
-        </is>
-      </c>
-      <c r="L155" s="53" t="inlineStr">
-        <is>
-          <t>No matching title in Tab3</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="53" t="inlineStr">
-        <is>
-          <t>원래 #13</t>
-        </is>
-      </c>
-      <c r="B156" s="53" t="inlineStr">
-        <is>
-          <t>10.51302/tce.2025.22219</t>
-        </is>
-      </c>
-      <c r="C156" s="53" t="inlineStr">
-        <is>
-          <t>Análisis sobre el uso de las herramientas de inteligencia artificial interactiva</t>
-        </is>
-      </c>
-      <c r="D156" s="53" t="n"/>
-      <c r="E156" s="53" t="n"/>
-      <c r="F156" s="53" t="n"/>
-      <c r="G156" s="53" t="n"/>
-      <c r="H156" s="53" t="n"/>
-      <c r="I156" s="53" t="n"/>
-      <c r="J156" s="53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K156" s="53" t="inlineStr">
-        <is>
-          <t>E-FT3</t>
-        </is>
-      </c>
-      <c r="L156" s="53" t="inlineStr">
-        <is>
-          <t>No matching title in Tab3</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="53" t="inlineStr">
-        <is>
-          <t>원래 #15</t>
-        </is>
-      </c>
-      <c r="B157" s="53" t="inlineStr">
-        <is>
-          <t>10.52142/omujecm.41.3.28</t>
-        </is>
-      </c>
-      <c r="C157" s="53" t="inlineStr">
-        <is>
-          <t>DOI not in CrossRef</t>
-        </is>
-      </c>
-      <c r="D157" s="53" t="n"/>
-      <c r="E157" s="53" t="n"/>
-      <c r="F157" s="53" t="n"/>
-      <c r="G157" s="53" t="n"/>
-      <c r="H157" s="53" t="n"/>
-      <c r="I157" s="53" t="n"/>
-      <c r="J157" s="53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K157" s="53" t="inlineStr">
-        <is>
-          <t>E-FT6</t>
-        </is>
-      </c>
-      <c r="L157" s="53" t="inlineStr">
-        <is>
-          <t>DOI not in CrossRef</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="53" t="inlineStr">
-        <is>
-          <t>원래 #56</t>
-        </is>
-      </c>
-      <c r="B158" s="53" t="inlineStr">
-        <is>
-          <t>10.32601/ejal.11210</t>
-        </is>
-      </c>
-      <c r="C158" s="53" t="inlineStr">
-        <is>
-          <t>DOI not in CrossRef</t>
-        </is>
-      </c>
-      <c r="D158" s="53" t="n"/>
-      <c r="E158" s="53" t="n"/>
-      <c r="F158" s="53" t="n"/>
-      <c r="G158" s="53" t="n"/>
-      <c r="H158" s="53" t="n"/>
-      <c r="I158" s="53" t="n"/>
-      <c r="J158" s="53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K158" s="53" t="inlineStr">
-        <is>
-          <t>E-FT1</t>
-        </is>
-      </c>
-      <c r="L158" s="53" t="inlineStr">
-        <is>
-          <t>DOI not in CrossRef</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:L152"/>

</xml_diff>